<commit_message>
Cleaned up a bit, added functions to extract LDTs
</commit_message>
<xml_diff>
--- a/src/test/resources/test-noproblems.xlsx
+++ b/src/test/resources/test-noproblems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mephistophilus\MyGitRepositories\ears3\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52467D57-44F3-4B21-9F1F-EF4B4D2B3552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4D90A8-B5A1-44E2-9B40-C644063C5331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="332" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1506,11 +1506,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1521,16 +1521,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1570,7 +1560,37 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1581,16 +1601,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1616,31 +1626,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1660,7 +1650,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1670,7 +1660,17 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1746,11 +1746,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1766,11 +1786,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1796,11 +1816,71 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1837,86 +1917,6 @@
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
@@ -2046,11 +2046,291 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2116,11 +2396,211 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2161,6 +2641,603 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2290,6 +3367,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -2326,11 +3413,241 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2351,6 +3668,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2416,16 +3753,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2441,6 +3768,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2476,21 +3843,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2521,346 +3888,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2916,11 +3943,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2936,11 +3963,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2976,63 +4003,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3048,976 +4018,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10405,11 +10405,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K53">
-    <cfRule type="cellIs" dxfId="254" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="201" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="199" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="201" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K31">
@@ -10428,14 +10428,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="249" priority="202" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="249" priority="204" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="248" priority="203" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="204" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="247" priority="202" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53">
@@ -10462,14 +10462,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K87">
-    <cfRule type="cellIs" dxfId="241" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="75" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="73" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="74" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="75" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:K128">
@@ -10488,22 +10488,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K155:K156 K158:K161">
-    <cfRule type="cellIs" dxfId="235" priority="1189" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="1191" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="1189" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="1191" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K167:K173">
-    <cfRule type="cellIs" dxfId="233" priority="925" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="233" priority="927" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="232" priority="926" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="927" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="231" priority="925" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K174">
@@ -10518,102 +10518,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K175:K182">
-    <cfRule type="cellIs" dxfId="227" priority="913" operator="equal">
-      <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="914" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="914" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="915" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="915" operator="equal">
       <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="913" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K183">
-    <cfRule type="cellIs" dxfId="224" priority="1138" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="224" priority="1140" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="223" priority="1139" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="1140" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="222" priority="1138" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K184:K193">
-    <cfRule type="cellIs" dxfId="221" priority="895" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="896" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="895" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="896" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="219" priority="897" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="cellIs" dxfId="218" priority="1024" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="1025" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="1024" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="1025" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="216" priority="1026" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195:K201">
-    <cfRule type="cellIs" dxfId="215" priority="847" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="848" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="847" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="848" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="213" priority="849" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202:K203">
-    <cfRule type="cellIs" dxfId="212" priority="1000" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="1002" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="1000" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="1001" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="1001" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="1002" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204:K210">
-    <cfRule type="cellIs" dxfId="209" priority="841" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="209" priority="843" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="208" priority="842" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="843" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="207" priority="841" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="cellIs" dxfId="206" priority="1126" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="1128" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="1126" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="1127" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="1127" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="1128" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212:K217 K236:K1048576">
-    <cfRule type="cellIs" dxfId="203" priority="1387" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1389" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="1387" operator="equal">
       <formula>"Interruption"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="1388" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1388" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="1389" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
@@ -10628,22 +10628,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219:K235">
-    <cfRule type="cellIs" dxfId="197" priority="829" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="830" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="829" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="830" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="195" priority="831" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
-    <cfRule type="cellIs" dxfId="194" priority="1150" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="1152" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="1150" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="1152" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L48 K133:L154 K127:L127 K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
@@ -10652,11 +10652,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L52">
-    <cfRule type="cellIs" dxfId="191" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="210" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="208" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="210" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:L36">
@@ -10670,25 +10670,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:L85">
-    <cfRule type="cellIs" dxfId="187" priority="37" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="187" priority="39" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="186" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="39" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="185" priority="37" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:L127">
-    <cfRule type="cellIs" dxfId="184" priority="7" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="184" priority="9" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="183" priority="8" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="9" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L134">
@@ -10697,11 +10697,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L154">
-    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="3" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="3" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K136:L139">
@@ -10710,80 +10710,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K166:L166">
-    <cfRule type="cellIs" dxfId="177" priority="262" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="177" priority="264" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="176" priority="263" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="264" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="175" priority="262" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L31">
-    <cfRule type="cellIs" dxfId="174" priority="214" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="174" priority="216" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="173" priority="215" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="216" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="172" priority="214" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L53">
-    <cfRule type="cellIs" dxfId="171" priority="196" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="171" priority="198" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="170" priority="197" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="198" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="169" priority="196" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:L87">
-    <cfRule type="cellIs" dxfId="168" priority="76" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="168" priority="78" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="167" priority="77" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="78" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="166" priority="76" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L128">
-    <cfRule type="cellIs" dxfId="165" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="165" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="164" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="163" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L138:L139">
     <cfRule type="cellIs" dxfId="162" priority="13" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="15" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="14" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="15" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L155:L156">
     <cfRule type="cellIs" dxfId="159" priority="259" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="261" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="260" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="261" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L236:L1048576">
@@ -22355,11 +22355,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA58">
-    <cfRule type="cellIs" dxfId="151" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="36" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="34" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="36" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AA36">
@@ -22378,14 +22378,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57">
-    <cfRule type="cellIs" dxfId="146" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="39" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="37" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="39" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA58">
@@ -22412,11 +22412,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA91:AA92">
-    <cfRule type="cellIs" dxfId="138" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="25" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="24" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="25" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="136" priority="26" operator="equal">
       <formula>"No impact"</formula>
@@ -22446,69 +22446,69 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA172:AA178">
-    <cfRule type="cellIs" dxfId="130" priority="71" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="130" priority="73" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="129" priority="72" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="73" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="128" priority="71" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA179">
-    <cfRule type="cellIs" dxfId="127" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="90" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="89" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="90" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="125" priority="91" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA180:AA187">
-    <cfRule type="cellIs" dxfId="124" priority="68" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="124" priority="70" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="123" priority="69" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="70" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="122" priority="68" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA188">
-    <cfRule type="cellIs" dxfId="121" priority="86" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="121" priority="88" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="120" priority="87" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="88" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="119" priority="86" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA189:AA198">
-    <cfRule type="cellIs" dxfId="118" priority="65" operator="equal">
-      <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="66" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="67" operator="equal">
       <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="65" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA199">
-    <cfRule type="cellIs" dxfId="115" priority="77" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="78" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="79" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="77" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA200:AA206">
@@ -22526,11 +22526,11 @@
     <cfRule type="cellIs" dxfId="109" priority="74" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="76" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="75" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="76" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA209:AA215">
@@ -22545,22 +22545,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA216">
-    <cfRule type="cellIs" dxfId="103" priority="83" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="103" priority="85" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="84" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="85" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA217:AA222 AA241:AA1048576">
-    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="102" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="101" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="102" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"No Impact"</formula>
@@ -22570,11 +22570,11 @@
     <cfRule type="cellIs" dxfId="97" priority="80" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="82" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="82" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA224:AA240">
@@ -22589,11 +22589,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
-    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="94" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="94" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB53 AA138:AB159 AA132:AB132 AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
@@ -22602,11 +22602,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB57">
-    <cfRule type="cellIs" dxfId="88" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="40" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA41:AB41">
@@ -22620,25 +22620,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA59:AB90">
-    <cfRule type="cellIs" dxfId="84" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="84" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="83" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA131:AB132">
-    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="81" priority="10" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB139">
@@ -22647,11 +22647,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB159">
-    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AB144">
@@ -22671,58 +22671,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB36">
-    <cfRule type="cellIs" dxfId="71" priority="44" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="46" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57:AB58">
-    <cfRule type="cellIs" dxfId="68" priority="31" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="68" priority="33" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="67" priority="32" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB91:AB92">
-    <cfRule type="cellIs" dxfId="65" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="28" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB133">
-    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="62" priority="19" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="61" priority="18" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="19" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="60" priority="17" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB143:AB144">
-    <cfRule type="cellIs" dxfId="59" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="14" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB160:AB161">
@@ -22805,8 +22805,8 @@
   <dimension ref="A1:AC147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28359,7 +28359,7 @@
         <v>315</v>
       </c>
       <c r="F86" s="58" t="s">
-        <v>291</v>
+        <v>333</v>
       </c>
       <c r="G86" s="36" t="s">
         <v>277</v>
@@ -32212,7 +32212,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="AA27:AA43 AA115 AB125 AA141:AA142 AA144:AA147 AA1:AA16 AA56:AA71 AA82:AA113 AA121:AA134">
+  <conditionalFormatting sqref="AA1:AA16 AA27:AA43 AA82:AA113 AA115 AA121:AA134 AB125 AA141:AA142 AA144:AA147">
     <cfRule type="cellIs" dxfId="50" priority="104" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
@@ -32240,25 +32240,25 @@
       <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AA47 AB148:AB1048576">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
-    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA72:AA81">
-    <cfRule type="cellIs" dxfId="43" priority="38" operator="equal">
+  <conditionalFormatting sqref="AA56:AA81">
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA80:AA81 AB1:AB26 AA49:AB79">
-    <cfRule type="cellIs" dxfId="42" priority="32" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="33" operator="equal">
-      <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="34" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA114:AA116">
@@ -32277,43 +32277,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AA142 AA144:AA147">
-    <cfRule type="cellIs" dxfId="36" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="105" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="103" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="105" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA148:AA1048576">
-    <cfRule type="cellIs" dxfId="34" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="80" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="79" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="80" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="32" priority="81" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA14:AB14 AA103:AA107 AB105 AB108 AA141:AA142 AA144:AB147 AA82:AB102 AA109 AA110:AB113 AA117:AB140">
-    <cfRule type="cellIs" dxfId="31" priority="100" operator="equal">
+  <conditionalFormatting sqref="AA14:AB14 AA82:AB102 AA103:AA107 AB105 AB108 AA109 AA117:AB140 AA141:AA142 AA144:AB147">
+    <cfRule type="cellIs" dxfId="31" priority="102" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="100" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="102" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA27:AB43 AA115:AB115 AA14:AB14 AA103:AA107 AB105 AB108 AA141:AA142 AA144:AB147 AA82:AB102 AA109 AA110:AB113 AA121:AB140">
+  <conditionalFormatting sqref="AA27:AB43 AA121:AB140 AA115:AB115 AA14:AB14 AA82:AB102 AA103:AA107 AB105 AB108 AA109 AA141:AA142 AA144:AB147">
     <cfRule type="cellIs" dxfId="29" priority="101" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AB47">
-    <cfRule type="cellIs" dxfId="28" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="50" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="48" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="50" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA31:AB31">
@@ -32326,7 +32326,7 @@
       <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA114:AB115">
+  <conditionalFormatting sqref="AA110:AB115">
     <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
@@ -32347,67 +32347,67 @@
       <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA47 AB148:AB1048576">
-    <cfRule type="cellIs" dxfId="19" priority="45" operator="equal">
-      <formula>"Heavy impact"</formula>
+  <conditionalFormatting sqref="AB1:AB26 AA49:AB79 AA80:AA81">
+    <cfRule type="cellIs" dxfId="19" priority="34" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="33" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="47" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="32" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB47:AB48">
-    <cfRule type="cellIs" dxfId="16" priority="39" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="41" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="41" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="14" priority="39" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB80:AB81">
-    <cfRule type="cellIs" dxfId="13" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="36" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="35" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="36" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB116">
-    <cfRule type="cellIs" dxfId="10" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB125">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB126:AB127">
-    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB141:AB142">

</xml_diff>

<commit_message>
Replaced error reporting with ErrorDTOList, added upload form, added constraint and reporting of constraintviolation
</commit_message>
<xml_diff>
--- a/src/test/resources/test-noproblems.xlsx
+++ b/src/test/resources/test-noproblems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mephistophilus\MyGitRepositories\ears3\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4D90A8-B5A1-44E2-9B40-C644063C5331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9319C377-47B5-4E8D-B028-6E9841749ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="332" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="332" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1314,7 +1314,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1467,6 +1467,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1506,11 +1509,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1521,6 +1524,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1560,7 +1573,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1570,7 +1583,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1581,26 +1594,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1626,11 +1619,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1650,7 +1663,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1660,17 +1673,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1746,16 +1749,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1770,7 +1763,27 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1791,26 +1804,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1841,6 +1834,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1896,16 +1899,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1921,6 +1914,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2046,291 +2049,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2396,211 +2119,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2641,603 +2164,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3367,16 +2293,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -3413,11 +2329,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3443,7 +2369,7 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -3467,17 +2393,17 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3543,11 +2469,361 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3593,11 +2869,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3624,6 +2900,363 @@
     <dxf>
       <font>
         <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -3677,17 +3310,77 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3753,6 +3446,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3768,46 +3471,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3843,21 +3506,21 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3888,6 +3551,346 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3943,11 +3946,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3963,11 +3966,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4003,21 +4006,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10405,11 +10408,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K53">
-    <cfRule type="cellIs" dxfId="254" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="199" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="201" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="199" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K31">
@@ -10428,14 +10431,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="249" priority="204" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="249" priority="202" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="248" priority="203" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="202" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="247" priority="204" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53">
@@ -10462,14 +10465,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K87">
-    <cfRule type="cellIs" dxfId="241" priority="75" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="73" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="74" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="239" priority="75" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:K128">
@@ -10488,22 +10491,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K155:K156 K158:K161">
-    <cfRule type="cellIs" dxfId="235" priority="1191" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="1189" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="1191" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="1189" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K167:K173">
-    <cfRule type="cellIs" dxfId="233" priority="927" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="233" priority="925" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="232" priority="926" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="925" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="231" priority="927" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K174">
@@ -10518,102 +10521,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K175:K182">
-    <cfRule type="cellIs" dxfId="227" priority="914" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="913" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="914" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="915" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="915" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="913" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K183">
-    <cfRule type="cellIs" dxfId="224" priority="1140" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="224" priority="1138" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="223" priority="1139" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="1138" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="222" priority="1140" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K184:K193">
-    <cfRule type="cellIs" dxfId="221" priority="896" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="895" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="896" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="895" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="219" priority="897" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="cellIs" dxfId="218" priority="1025" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="1024" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="1025" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="1024" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="216" priority="1026" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195:K201">
-    <cfRule type="cellIs" dxfId="215" priority="848" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="847" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="848" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="847" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="213" priority="849" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202:K203">
-    <cfRule type="cellIs" dxfId="212" priority="1002" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="1000" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="1000" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="1001" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="1001" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="1002" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204:K210">
-    <cfRule type="cellIs" dxfId="209" priority="843" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="209" priority="841" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="208" priority="842" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="841" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="207" priority="843" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="cellIs" dxfId="206" priority="1128" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="1126" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="1126" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="1127" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="1127" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="204" priority="1128" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212:K217 K236:K1048576">
-    <cfRule type="cellIs" dxfId="203" priority="1389" operator="equal">
-      <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="1387" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1387" operator="equal">
       <formula>"Interruption"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="1388" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="1388" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="1389" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
@@ -10628,22 +10631,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219:K235">
-    <cfRule type="cellIs" dxfId="197" priority="830" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="829" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="830" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="829" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="195" priority="831" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
-    <cfRule type="cellIs" dxfId="194" priority="1152" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="1150" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="1152" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="1150" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L48 K133:L154 K127:L127 K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
@@ -10652,11 +10655,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L52">
-    <cfRule type="cellIs" dxfId="191" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="208" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="210" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="208" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:L36">
@@ -10670,25 +10673,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:L85">
-    <cfRule type="cellIs" dxfId="187" priority="39" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="187" priority="37" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="186" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="37" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="185" priority="39" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:L127">
-    <cfRule type="cellIs" dxfId="184" priority="9" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="184" priority="7" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="183" priority="8" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="182" priority="9" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L134">
@@ -10697,11 +10700,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L154">
-    <cfRule type="cellIs" dxfId="180" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="3" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K136:L139">
@@ -10710,80 +10713,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K166:L166">
-    <cfRule type="cellIs" dxfId="177" priority="264" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="177" priority="262" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="176" priority="263" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="262" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="175" priority="264" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L31">
-    <cfRule type="cellIs" dxfId="174" priority="216" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="174" priority="214" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="173" priority="215" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="214" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="172" priority="216" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L53">
-    <cfRule type="cellIs" dxfId="171" priority="198" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="171" priority="196" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="170" priority="197" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="196" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="169" priority="198" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:L87">
-    <cfRule type="cellIs" dxfId="168" priority="78" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="168" priority="76" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="167" priority="77" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="76" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="166" priority="78" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L128">
-    <cfRule type="cellIs" dxfId="165" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="165" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="164" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="163" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L138:L139">
     <cfRule type="cellIs" dxfId="162" priority="13" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="14" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="15" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="14" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L155:L156">
     <cfRule type="cellIs" dxfId="159" priority="259" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="260" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="261" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="260" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L236:L1048576">
@@ -22355,11 +22358,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA58">
-    <cfRule type="cellIs" dxfId="151" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="34" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="36" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="34" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AA36">
@@ -22378,14 +22381,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57">
-    <cfRule type="cellIs" dxfId="146" priority="39" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="37" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="39" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA58">
@@ -22412,11 +22415,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA91:AA92">
-    <cfRule type="cellIs" dxfId="138" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="24" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="25" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="24" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="136" priority="26" operator="equal">
       <formula>"No impact"</formula>
@@ -22446,69 +22449,69 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA172:AA178">
-    <cfRule type="cellIs" dxfId="130" priority="73" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="130" priority="71" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="129" priority="72" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="71" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="128" priority="73" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA179">
-    <cfRule type="cellIs" dxfId="127" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="89" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="90" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="89" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="125" priority="91" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA180:AA187">
-    <cfRule type="cellIs" dxfId="124" priority="70" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="124" priority="68" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="123" priority="69" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="68" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="122" priority="70" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA188">
-    <cfRule type="cellIs" dxfId="121" priority="88" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="121" priority="86" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="120" priority="87" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="86" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="119" priority="88" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA189:AA198">
-    <cfRule type="cellIs" dxfId="118" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="65" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="66" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="67" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="65" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA199">
-    <cfRule type="cellIs" dxfId="115" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="77" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="78" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="79" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="77" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA200:AA206">
@@ -22526,11 +22529,11 @@
     <cfRule type="cellIs" dxfId="109" priority="74" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="75" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="76" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="75" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA209:AA215">
@@ -22545,22 +22548,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA216">
-    <cfRule type="cellIs" dxfId="103" priority="85" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="103" priority="83" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="84" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="83" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="101" priority="85" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA217:AA222 AA241:AA1048576">
-    <cfRule type="cellIs" dxfId="100" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="102" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="101" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"No Impact"</formula>
@@ -22570,11 +22573,11 @@
     <cfRule type="cellIs" dxfId="97" priority="80" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="81" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="82" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA224:AA240">
@@ -22589,11 +22592,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
-    <cfRule type="cellIs" dxfId="91" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="94" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB53 AA138:AB159 AA132:AB132 AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
@@ -22602,11 +22605,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB57">
-    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="40" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="40" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA41:AB41">
@@ -22620,25 +22623,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA59:AB90">
-    <cfRule type="cellIs" dxfId="84" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="84" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="83" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="82" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA131:AB132">
-    <cfRule type="cellIs" dxfId="81" priority="10" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB139">
@@ -22647,11 +22650,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB159">
-    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AB144">
@@ -22671,58 +22674,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB36">
-    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="44" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="45" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="46" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57:AB58">
-    <cfRule type="cellIs" dxfId="68" priority="33" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="68" priority="31" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="67" priority="32" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB91:AB92">
-    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="27" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="28" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB133">
-    <cfRule type="cellIs" dxfId="62" priority="19" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="61" priority="18" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="17" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="60" priority="19" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB143:AB144">
-    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
-      <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="12" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
       <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="14" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB160:AB161">
@@ -22805,8 +22808,8 @@
   <dimension ref="A1:AC147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22928,7 +22931,7 @@
       <c r="E2" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="68" t="s">
         <v>332</v>
       </c>
       <c r="G2" s="36" t="s">
@@ -22989,7 +22992,7 @@
       <c r="E3" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="68" t="s">
         <v>332</v>
       </c>
       <c r="G3" s="36" t="s">
@@ -23111,7 +23114,7 @@
       <c r="E5" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F5" s="65" t="s">
+      <c r="F5" s="68" t="s">
         <v>332</v>
       </c>
       <c r="G5" s="37" t="s">
@@ -23288,7 +23291,7 @@
       <c r="E8" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="68" t="s">
         <v>332</v>
       </c>
       <c r="G8" s="36" t="s">
@@ -25382,7 +25385,7 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="33">
-        <v>45207</v>
+        <v>45208</v>
       </c>
       <c r="B39" s="43">
         <v>2.0833333333333332E-2</v>
@@ -32241,14 +32244,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA47 AB148:AB1048576">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
@@ -32277,30 +32280,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AA142 AA144:AA147">
-    <cfRule type="cellIs" dxfId="36" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="103" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="105" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="103" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA148:AA1048576">
-    <cfRule type="cellIs" dxfId="34" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="79" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="80" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="79" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="32" priority="81" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14:AB14 AA82:AB102 AA103:AA107 AB105 AB108 AA109 AA117:AB140 AA141:AA142 AA144:AB147">
-    <cfRule type="cellIs" dxfId="31" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="100" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="102" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="100" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AB43 AA121:AB140 AA115:AB115 AA14:AB14 AA82:AB102 AA103:AA107 AB105 AB108 AA109 AA141:AA142 AA144:AB147">
@@ -32309,11 +32312,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AB47">
-    <cfRule type="cellIs" dxfId="28" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="48" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="50" operator="equal">
       <formula>"No impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="48" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA31:AB31">
@@ -32348,66 +32351,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AB26 AA49:AB79 AA80:AA81">
-    <cfRule type="cellIs" dxfId="19" priority="34" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="32" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="33" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="32" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="34" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB47:AB48">
-    <cfRule type="cellIs" dxfId="16" priority="41" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="39" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="39" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="14" priority="41" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB80:AB81">
-    <cfRule type="cellIs" dxfId="13" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="35" operator="equal">
+      <formula>"Heavy impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="36" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="35" operator="equal">
-      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB116">
-    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="10" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB125">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+      <formula>"Interruption"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>"No Impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
-      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB126:AB127">
-    <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB141:AB142">

</xml_diff>

<commit_message>
Added the Remarks field to Event, EventDTO, the services for Event and Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test-noproblems.xlsx
+++ b/src/test/resources/test-noproblems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mephistophilus\MyGitRepositories\ears3\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9319C377-47B5-4E8D-B028-6E9841749ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04F5179-580A-410B-B3EF-EB612D17E1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="332" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5029" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5030" uniqueCount="335">
   <si>
     <t>Date</t>
   </si>
@@ -1089,6 +1089,9 @@
   </si>
   <si>
     <t>Unknown sparker</t>
+  </si>
+  <si>
+    <t>Laten we zien of dit ook opgepikt wordt</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1317,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1467,9 +1470,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1509,11 +1509,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1524,16 +1524,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1573,7 +1563,37 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1584,16 +1604,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1619,31 +1629,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1663,7 +1653,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1673,7 +1663,17 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1749,11 +1749,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1769,11 +1789,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1794,16 +1814,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1834,16 +1844,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1899,6 +1899,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1914,16 +1924,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2049,11 +2049,291 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2119,11 +2399,211 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2164,6 +2644,603 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2293,6 +3370,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -2329,11 +3416,241 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2354,6 +3671,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2419,16 +3756,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2444,6 +3771,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2479,21 +3846,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2524,346 +3891,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2919,11 +3946,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2939,11 +3966,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2979,63 +4006,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3051,976 +4021,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10408,11 +10408,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K53">
-    <cfRule type="cellIs" dxfId="254" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="201" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="199" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="201" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K31">
@@ -10431,14 +10431,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="249" priority="202" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="249" priority="204" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="248" priority="203" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="204" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="247" priority="202" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53">
@@ -10465,14 +10465,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K87">
-    <cfRule type="cellIs" dxfId="241" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="75" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="73" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="74" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="75" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:K128">
@@ -10491,22 +10491,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K155:K156 K158:K161">
-    <cfRule type="cellIs" dxfId="235" priority="1189" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="1191" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="1189" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="1191" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K167:K173">
-    <cfRule type="cellIs" dxfId="233" priority="925" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="233" priority="927" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="232" priority="926" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="927" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="231" priority="925" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K174">
@@ -10521,102 +10521,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K175:K182">
-    <cfRule type="cellIs" dxfId="227" priority="913" operator="equal">
-      <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="914" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="914" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="915" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="915" operator="equal">
       <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="913" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K183">
-    <cfRule type="cellIs" dxfId="224" priority="1138" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="224" priority="1140" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="223" priority="1139" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="1140" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="222" priority="1138" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K184:K193">
-    <cfRule type="cellIs" dxfId="221" priority="895" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="896" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="895" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="896" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="219" priority="897" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="cellIs" dxfId="218" priority="1024" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="1025" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="1024" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="1025" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="216" priority="1026" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195:K201">
-    <cfRule type="cellIs" dxfId="215" priority="847" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="848" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="847" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="848" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="213" priority="849" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202:K203">
-    <cfRule type="cellIs" dxfId="212" priority="1000" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="1002" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="1000" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="1001" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="1001" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="1002" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204:K210">
-    <cfRule type="cellIs" dxfId="209" priority="841" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="209" priority="843" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="208" priority="842" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="843" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="207" priority="841" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="cellIs" dxfId="206" priority="1126" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="1128" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="1126" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="1127" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="1127" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="1128" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212:K217 K236:K1048576">
-    <cfRule type="cellIs" dxfId="203" priority="1387" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1389" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="1387" operator="equal">
       <formula>"Interruption"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="1388" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1388" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="1389" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
@@ -10631,22 +10631,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219:K235">
-    <cfRule type="cellIs" dxfId="197" priority="829" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="830" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="829" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="830" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="195" priority="831" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
-    <cfRule type="cellIs" dxfId="194" priority="1150" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="1152" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="1150" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="1152" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L48 K133:L154 K127:L127 K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
@@ -10655,11 +10655,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L52">
-    <cfRule type="cellIs" dxfId="191" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="210" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="208" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="210" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:L36">
@@ -10673,25 +10673,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:L85">
-    <cfRule type="cellIs" dxfId="187" priority="37" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="187" priority="39" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="186" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="39" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="185" priority="37" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:L127">
-    <cfRule type="cellIs" dxfId="184" priority="7" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="184" priority="9" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="183" priority="8" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="9" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L134">
@@ -10700,11 +10700,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L154">
-    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="3" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="3" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K136:L139">
@@ -10713,80 +10713,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K166:L166">
-    <cfRule type="cellIs" dxfId="177" priority="262" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="177" priority="264" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="176" priority="263" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="264" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="175" priority="262" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L31">
-    <cfRule type="cellIs" dxfId="174" priority="214" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="174" priority="216" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="173" priority="215" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="216" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="172" priority="214" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L53">
-    <cfRule type="cellIs" dxfId="171" priority="196" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="171" priority="198" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="170" priority="197" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="198" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="169" priority="196" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:L87">
-    <cfRule type="cellIs" dxfId="168" priority="76" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="168" priority="78" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="167" priority="77" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="78" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="166" priority="76" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L128">
-    <cfRule type="cellIs" dxfId="165" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="165" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="164" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="163" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L138:L139">
     <cfRule type="cellIs" dxfId="162" priority="13" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="15" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="14" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="15" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L155:L156">
     <cfRule type="cellIs" dxfId="159" priority="259" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="261" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="260" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="261" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L236:L1048576">
@@ -22358,11 +22358,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA58">
-    <cfRule type="cellIs" dxfId="151" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="36" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="34" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="36" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AA36">
@@ -22381,14 +22381,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57">
-    <cfRule type="cellIs" dxfId="146" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="39" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="37" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="39" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA58">
@@ -22415,11 +22415,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA91:AA92">
-    <cfRule type="cellIs" dxfId="138" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="25" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="24" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="25" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="136" priority="26" operator="equal">
       <formula>"No impact"</formula>
@@ -22449,69 +22449,69 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA172:AA178">
-    <cfRule type="cellIs" dxfId="130" priority="71" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="130" priority="73" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="129" priority="72" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="73" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="128" priority="71" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA179">
-    <cfRule type="cellIs" dxfId="127" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="90" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="89" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="90" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="125" priority="91" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA180:AA187">
-    <cfRule type="cellIs" dxfId="124" priority="68" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="124" priority="70" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="123" priority="69" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="70" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="122" priority="68" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA188">
-    <cfRule type="cellIs" dxfId="121" priority="86" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="121" priority="88" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="120" priority="87" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="88" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="119" priority="86" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA189:AA198">
-    <cfRule type="cellIs" dxfId="118" priority="65" operator="equal">
-      <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="66" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="67" operator="equal">
       <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="65" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA199">
-    <cfRule type="cellIs" dxfId="115" priority="77" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="78" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="79" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="77" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA200:AA206">
@@ -22529,11 +22529,11 @@
     <cfRule type="cellIs" dxfId="109" priority="74" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="76" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="75" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="76" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA209:AA215">
@@ -22548,22 +22548,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA216">
-    <cfRule type="cellIs" dxfId="103" priority="83" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="103" priority="85" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="84" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="85" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA217:AA222 AA241:AA1048576">
-    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="102" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="101" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="102" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"No Impact"</formula>
@@ -22573,11 +22573,11 @@
     <cfRule type="cellIs" dxfId="97" priority="80" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="82" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="82" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA224:AA240">
@@ -22592,11 +22592,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
-    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="94" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="94" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB53 AA138:AB159 AA132:AB132 AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
@@ -22605,11 +22605,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB57">
-    <cfRule type="cellIs" dxfId="88" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="40" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA41:AB41">
@@ -22623,25 +22623,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA59:AB90">
-    <cfRule type="cellIs" dxfId="84" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="84" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="83" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA131:AB132">
-    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="81" priority="10" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB139">
@@ -22650,11 +22650,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB159">
-    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AB144">
@@ -22674,58 +22674,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB36">
-    <cfRule type="cellIs" dxfId="71" priority="44" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="46" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57:AB58">
-    <cfRule type="cellIs" dxfId="68" priority="31" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="68" priority="33" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="67" priority="32" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB91:AB92">
-    <cfRule type="cellIs" dxfId="65" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="28" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB133">
-    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="62" priority="19" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="61" priority="18" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="19" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="60" priority="17" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB143:AB144">
-    <cfRule type="cellIs" dxfId="59" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="14" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB160:AB161">
@@ -22809,7 +22809,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22931,7 +22931,7 @@
       <c r="E2" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="65" t="s">
         <v>332</v>
       </c>
       <c r="G2" s="36" t="s">
@@ -22992,7 +22992,7 @@
       <c r="E3" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="65" t="s">
         <v>332</v>
       </c>
       <c r="G3" s="36" t="s">
@@ -23114,7 +23114,7 @@
       <c r="E5" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="65" t="s">
         <v>332</v>
       </c>
       <c r="G5" s="37" t="s">
@@ -23291,7 +23291,7 @@
       <c r="E8" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="65" t="s">
         <v>332</v>
       </c>
       <c r="G8" s="36" t="s">
@@ -23857,7 +23857,9 @@
         <v>79</v>
       </c>
       <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
+      <c r="L16" s="37" t="s">
+        <v>334</v>
+      </c>
       <c r="M16" s="37"/>
       <c r="N16" s="37"/>
       <c r="O16" s="37"/>
@@ -32244,14 +32246,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA47 AB148:AB1048576">
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
@@ -32280,30 +32282,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AA142 AA144:AA147">
-    <cfRule type="cellIs" dxfId="36" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="105" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="103" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="105" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA148:AA1048576">
-    <cfRule type="cellIs" dxfId="34" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="80" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="79" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="80" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="32" priority="81" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14:AB14 AA82:AB102 AA103:AA107 AB105 AB108 AA109 AA117:AB140 AA141:AA142 AA144:AB147">
-    <cfRule type="cellIs" dxfId="31" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="102" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="100" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="102" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AB43 AA121:AB140 AA115:AB115 AA14:AB14 AA82:AB102 AA103:AA107 AB105 AB108 AA109 AA141:AA142 AA144:AB147">
@@ -32312,11 +32314,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AB47">
-    <cfRule type="cellIs" dxfId="28" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="50" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="48" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="50" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA31:AB31">
@@ -32351,66 +32353,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AB26 AA49:AB79 AA80:AA81">
-    <cfRule type="cellIs" dxfId="19" priority="32" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="34" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="33" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="34" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="32" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB47:AB48">
-    <cfRule type="cellIs" dxfId="16" priority="39" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="41" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="41" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="14" priority="39" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB80:AB81">
-    <cfRule type="cellIs" dxfId="13" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="36" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="35" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="36" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB116">
-    <cfRule type="cellIs" dxfId="10" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB125">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB126:AB127">
-    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB141:AB142">

</xml_diff>